<commit_message>
Modify and Improve Generate Report Logic
</commit_message>
<xml_diff>
--- a/App_Admin/temp/p_assessment_number_df.xlsx
+++ b/App_Admin/temp/p_assessment_number_df.xlsx
@@ -457,21 +457,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anantara_Analytics</t>
+          <t>Hogwarts</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NeuCode</t>
+          <t>Gryffindoar</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>180</t>
         </is>
       </c>
     </row>

</xml_diff>